<commit_message>
Banner Home + Đa Ngôn Ngữ
</commit_message>
<xml_diff>
--- a/docs/DaNgonNgu_20140621.xlsx
+++ b/docs/DaNgonNgu_20140621.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="197">
   <si>
     <t>Tiếng Việt</t>
   </si>
@@ -291,9 +291,6 @@
     <t xml:space="preserve">마이 카트 </t>
   </si>
   <si>
-    <t>(My Cart)</t>
-  </si>
-  <si>
     <t>HOT 상품</t>
   </si>
   <si>
@@ -568,6 +565,54 @@
   </si>
   <si>
     <t>합계금액</t>
+  </si>
+  <si>
+    <t>카테고리 전체</t>
+  </si>
+  <si>
+    <t xml:space="preserve">마이 장바구니 </t>
+  </si>
+  <si>
+    <t>유아동</t>
+  </si>
+  <si>
+    <t>전체보기</t>
+  </si>
+  <si>
+    <t>BEST 상품</t>
+  </si>
+  <si>
+    <t>오늘의 핫딜</t>
+  </si>
+  <si>
+    <t>전통의류</t>
+  </si>
+  <si>
+    <t>찜</t>
+  </si>
+  <si>
+    <t>공유하기</t>
+  </si>
+  <si>
+    <t>품질보증 &amp; 반품</t>
+  </si>
+  <si>
+    <t>총 합계금액</t>
+  </si>
+  <si>
+    <t>삭제하기</t>
+  </si>
+  <si>
+    <t>Wishlist 으로 이동</t>
+  </si>
+  <si>
+    <t>주문하실 상품</t>
+  </si>
+  <si>
+    <t>결제하기</t>
+  </si>
+  <si>
+    <t>Chỉnh</t>
   </si>
 </sst>
 </file>
@@ -917,15 +962,16 @@
   </sheetPr>
   <dimension ref="B3:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.140625" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
@@ -938,6 +984,9 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -947,7 +996,10 @@
         <v>83</v>
       </c>
       <c r="D5" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="E5" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -960,6 +1012,9 @@
       <c r="D6" t="s">
         <v>84</v>
       </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -971,6 +1026,9 @@
       <c r="D7" t="s">
         <v>85</v>
       </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -982,10 +1040,13 @@
       <c r="D8" t="s">
         <v>86</v>
       </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="2:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>10</v>
@@ -993,10 +1054,13 @@
       <c r="D9" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="E9" s="2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1004,10 +1068,13 @@
       <c r="D10" t="s">
         <v>87</v>
       </c>
+      <c r="E10" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1016,7 +1083,7 @@
         <v>88</v>
       </c>
       <c r="E11" t="s">
-        <v>89</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1027,7 +1094,10 @@
         <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1038,7 +1108,10 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1049,7 +1122,10 @@
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
@@ -1060,10 +1136,13 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>17</v>
       </c>
@@ -1071,10 +1150,13 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="E17" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -1082,10 +1164,13 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -1093,10 +1178,13 @@
         <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -1104,7 +1192,10 @@
         <v>16</v>
       </c>
       <c r="D20" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="E20" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1117,20 +1208,21 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B3:D16"/>
+  <dimension ref="B3:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1140,8 +1232,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>44</v>
       </c>
@@ -1149,10 +1244,13 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>53</v>
       </c>
@@ -1160,10 +1258,13 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="E6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>54</v>
       </c>
@@ -1171,10 +1272,13 @@
         <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="E7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>55</v>
       </c>
@@ -1182,10 +1286,13 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>45</v>
       </c>
@@ -1193,10 +1300,13 @@
         <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>48</v>
       </c>
@@ -1206,19 +1316,25 @@
       <c r="D10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>49</v>
       </c>
@@ -1226,32 +1342,41 @@
         <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="E13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="E14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>51</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="E15" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>52</v>
       </c>
@@ -1259,7 +1384,10 @@
         <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>154</v>
+        <v>153</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1272,10 +1400,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B3:D7"/>
+  <dimension ref="B3:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,9 +1411,10 @@
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1295,8 +1424,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>64</v>
       </c>
@@ -1304,10 +1436,13 @@
         <v>69</v>
       </c>
       <c r="D5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="E5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>65</v>
       </c>
@@ -1315,10 +1450,13 @@
         <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="E6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>66</v>
       </c>
@@ -1326,7 +1464,10 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>145</v>
+      </c>
+      <c r="E7" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1339,10 +1480,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B3:D9"/>
+  <dimension ref="B3:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1350,9 +1491,10 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1362,8 +1504,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>70</v>
       </c>
@@ -1371,10 +1516,13 @@
         <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>71</v>
       </c>
@@ -1382,10 +1530,13 @@
         <v>79</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="E6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>72</v>
       </c>
@@ -1393,10 +1544,13 @@
         <v>76</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>73</v>
       </c>
@@ -1404,10 +1558,13 @@
         <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>74</v>
       </c>
@@ -1415,7 +1572,10 @@
         <v>78</v>
       </c>
       <c r="D9" t="s">
-        <v>153</v>
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1428,10 +1588,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B3:D6"/>
+  <dimension ref="B3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,9 +1599,10 @@
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1451,8 +1612,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>80</v>
       </c>
@@ -1460,10 +1624,13 @@
         <v>82</v>
       </c>
       <c r="D5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="E5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>81</v>
       </c>
@@ -1471,7 +1638,10 @@
         <v>81</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>151</v>
+      </c>
+      <c r="E6" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1484,10 +1654,10 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B3:D17"/>
+  <dimension ref="B3:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,9 +1665,10 @@
     <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.140625" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1507,8 +1678,11 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -1516,10 +1690,13 @@
         <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -1527,10 +1704,13 @@
         <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>36</v>
       </c>
@@ -1538,10 +1718,13 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>35</v>
       </c>
@@ -1549,10 +1732,13 @@
         <v>30</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="E9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -1560,10 +1746,13 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+      <c r="E10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>34</v>
       </c>
@@ -1571,10 +1760,13 @@
         <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="E11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>40</v>
       </c>
@@ -1582,21 +1774,27 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>99</v>
-      </c>
-      <c r="C13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D13" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -1604,10 +1802,13 @@
         <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="E15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>27</v>
       </c>
@@ -1615,10 +1816,13 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="E16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
@@ -1626,7 +1830,10 @@
         <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>161</v>
+      </c>
+      <c r="E17" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -1636,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E23"/>
+  <dimension ref="B2:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,9 +1854,10 @@
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1659,206 +1867,263 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
         <v>105</v>
       </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="D5" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
         <v>107</v>
       </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="D6" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="F6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
         <v>109</v>
       </c>
-      <c r="C6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="F7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" t="s">
         <v>111</v>
       </c>
-      <c r="C7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="F9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>180</v>
+      </c>
+      <c r="F10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" t="s">
+        <v>172</v>
+      </c>
+      <c r="F11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F14" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="F17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
         <v>113</v>
       </c>
-      <c r="C8" t="s">
-        <v>112</v>
-      </c>
-      <c r="D8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D20" t="s">
+        <v>169</v>
+      </c>
+      <c r="F20" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
         <v>114</v>
       </c>
-      <c r="D9" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F22" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
         <v>131</v>
       </c>
-      <c r="C10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D23" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>122</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C17" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>126</v>
-      </c>
-      <c r="C18" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>116</v>
-      </c>
-      <c r="C20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D22" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" t="s">
-        <v>132</v>
-      </c>
-      <c r="D23" t="s">
-        <v>178</v>
+      <c r="F23" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Đa ngôn ngữ - Billing Address
</commit_message>
<xml_diff>
--- a/docs/DaNgonNgu_20140621.xlsx
+++ b/docs/DaNgonNgu_20140621.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="254">
   <si>
     <t>Tiếng Việt</t>
   </si>
@@ -613,6 +613,177 @@
   </si>
   <si>
     <t>Chỉnh</t>
+  </si>
+  <si>
+    <t>Địa chỉ nhận hàng</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>수령주소</t>
+  </si>
+  <si>
+    <t>주문자 정보</t>
+  </si>
+  <si>
+    <t>Họ và Tên</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>성명</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>휴대전화</t>
+  </si>
+  <si>
+    <t>Địa chỉ</t>
+  </si>
+  <si>
+    <t>Street Address</t>
+  </si>
+  <si>
+    <t>주소</t>
+  </si>
+  <si>
+    <t>Thành Phố</t>
+  </si>
+  <si>
+    <t>City/District</t>
+  </si>
+  <si>
+    <t>시</t>
+  </si>
+  <si>
+    <t>Tỉnh</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>성</t>
+  </si>
+  <si>
+    <t>Phương Thức Vận Chuyển</t>
+  </si>
+  <si>
+    <t>Shipping Methods</t>
+  </si>
+  <si>
+    <t>배송방법</t>
+  </si>
+  <si>
+    <t>Loại</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Thời gian vận chuyển</t>
+  </si>
+  <si>
+    <t>Shipping Time</t>
+  </si>
+  <si>
+    <t>배송기간</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thông thường </t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>일반</t>
+  </si>
+  <si>
+    <t>3-5 ngày (không tính cuối tuần)</t>
+  </si>
+  <si>
+    <t>3-5 business days</t>
+  </si>
+  <si>
+    <t>3~5일 (토, 일, 휴무일, 공휴일 제외)</t>
+  </si>
+  <si>
+    <t>Nhanh</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>프리미음</t>
+  </si>
+  <si>
+    <t>1-3 ngày (không tính cuối tuần)</t>
+  </si>
+  <si>
+    <t>1-3 business days</t>
+  </si>
+  <si>
+    <t>1~3일 (토, 일 휴무일, 공휴일 제외)</t>
+  </si>
+  <si>
+    <t>Rất nhanh</t>
+  </si>
+  <si>
+    <t>Express</t>
+  </si>
+  <si>
+    <t>익스프레스</t>
+  </si>
+  <si>
+    <t>Trong ngày (không tính cuối tuần)</t>
+  </si>
+  <si>
+    <t>하루 이내 (토, 일 휴무일, 공휴일 제외)</t>
+  </si>
+  <si>
+    <t>Gói Quà</t>
+  </si>
+  <si>
+    <t>Gift Option</t>
+  </si>
+  <si>
+    <t>선물꾸러미</t>
+  </si>
+  <si>
+    <t>Sản phẩm làm quà tặng</t>
+  </si>
+  <si>
+    <t>This order is a gift</t>
+  </si>
+  <si>
+    <t>이 상품은 선물입니다</t>
+  </si>
+  <si>
+    <t>Không phải là quà tặng</t>
+  </si>
+  <si>
+    <t>Not a gift</t>
+  </si>
+  <si>
+    <t>이 상품은 선물이 아닙니다</t>
+  </si>
+  <si>
+    <t>Trở về giỏ hàng</t>
+  </si>
+  <si>
+    <t>Back to cart</t>
+  </si>
+  <si>
+    <t>장바구니로</t>
+  </si>
+  <si>
+    <t>Within a  (Exept weekends)</t>
   </si>
 </sst>
 </file>
@@ -963,7 +1134,7 @@
   <dimension ref="B3:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1827,7 @@
   </sheetPr>
   <dimension ref="B3:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -2164,12 +2335,242 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" t="s">
+        <v>198</v>
+      </c>
+      <c r="D4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" t="s">
+        <v>205</v>
+      </c>
+      <c r="D7" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C8" t="s">
+        <v>208</v>
+      </c>
+      <c r="D8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C10" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>224</v>
+      </c>
+      <c r="C16" t="s">
+        <v>225</v>
+      </c>
+      <c r="D16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" t="s">
+        <v>231</v>
+      </c>
+      <c r="D18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>236</v>
+      </c>
+      <c r="C20" t="s">
+        <v>237</v>
+      </c>
+      <c r="D20" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C21" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C23" t="s">
+        <v>242</v>
+      </c>
+      <c r="D23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>244</v>
+      </c>
+      <c r="C24" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>247</v>
+      </c>
+      <c r="C25" t="s">
+        <v>248</v>
+      </c>
+      <c r="D25" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>250</v>
+      </c>
+      <c r="C27" t="s">
+        <v>251</v>
+      </c>
+      <c r="D27" t="s">
+        <v>252</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>